<commit_message>
updated create_xlsx_group_x_variable and create_xlsx_variable_x_group
</commit_message>
<xml_diff>
--- a/outputs/04 - example - group_x_variable.xlsx
+++ b/outputs/04 - example - group_x_variable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/tomas_beyene_reach-initiative_org/Documents/Documents/IMPACT_R_FRAMEWORK_EXERCISE/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_96EED235FE5163C764B882F84F90A9F3CFA8F4D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27AFA6E3-13FD-41BC-97AE-725E5C0F9AB1}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_96EED235FE5163C764B882F84F90A9F3CFA8F4D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D89B3A-17DF-4A5A-8465-D9FCA715DA8C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_group_x_variable" sheetId="1" r:id="rId1"/>
@@ -851,15 +851,17 @@
   <dimension ref="A1:QU10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="QM5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AD5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="QR11" sqref="QR11"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="323" max="325" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="326" max="326" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="457" max="457" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14439,6 +14441,79 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="T3:AE3"/>
+    <mergeCell ref="AF1:AT1"/>
+    <mergeCell ref="AF3:AT3"/>
+    <mergeCell ref="AU1:BI1"/>
+    <mergeCell ref="AU3:BI3"/>
+    <mergeCell ref="BJ1:BX1"/>
+    <mergeCell ref="BJ3:BX3"/>
+    <mergeCell ref="BY1:CV1"/>
+    <mergeCell ref="BY3:CV3"/>
+    <mergeCell ref="CW1:DT1"/>
+    <mergeCell ref="CW3:DT3"/>
+    <mergeCell ref="DU1:ER1"/>
+    <mergeCell ref="DU3:ER3"/>
+    <mergeCell ref="ES1:FP1"/>
+    <mergeCell ref="ES3:FP3"/>
+    <mergeCell ref="FQ1:GN1"/>
+    <mergeCell ref="FQ3:GN3"/>
+    <mergeCell ref="GO1:GZ1"/>
+    <mergeCell ref="GO3:GZ3"/>
+    <mergeCell ref="HA1:HL1"/>
+    <mergeCell ref="HA3:HL3"/>
+    <mergeCell ref="HM1:HX1"/>
+    <mergeCell ref="HM3:HX3"/>
+    <mergeCell ref="HY1:IJ1"/>
+    <mergeCell ref="HY3:IJ3"/>
+    <mergeCell ref="IK1:IV1"/>
+    <mergeCell ref="IK3:IV3"/>
+    <mergeCell ref="IW1:JH1"/>
+    <mergeCell ref="IW3:JH3"/>
+    <mergeCell ref="JI1:JT1"/>
+    <mergeCell ref="JI3:JT3"/>
+    <mergeCell ref="JU1:KF1"/>
+    <mergeCell ref="JU3:KF3"/>
+    <mergeCell ref="KG1:KR1"/>
+    <mergeCell ref="KG3:KR3"/>
+    <mergeCell ref="KS1:LD1"/>
+    <mergeCell ref="KS3:LD3"/>
+    <mergeCell ref="LE1:LJ1"/>
+    <mergeCell ref="LE3:LJ3"/>
+    <mergeCell ref="LK1:LV1"/>
+    <mergeCell ref="LK3:LV3"/>
+    <mergeCell ref="LW1:MB1"/>
+    <mergeCell ref="LW3:MB3"/>
+    <mergeCell ref="MC1:MN1"/>
+    <mergeCell ref="MC3:MN3"/>
+    <mergeCell ref="MO1:MT1"/>
+    <mergeCell ref="MO3:MT3"/>
+    <mergeCell ref="MU1:NF1"/>
+    <mergeCell ref="MU3:NF3"/>
+    <mergeCell ref="NG1:OY1"/>
+    <mergeCell ref="NG3:OY3"/>
+    <mergeCell ref="OZ1:PB1"/>
+    <mergeCell ref="OZ3:PB3"/>
+    <mergeCell ref="PC1:PE1"/>
+    <mergeCell ref="PC3:PE3"/>
+    <mergeCell ref="PF1:PH1"/>
+    <mergeCell ref="PF3:PH3"/>
+    <mergeCell ref="PI1:PK1"/>
+    <mergeCell ref="PI3:PK3"/>
+    <mergeCell ref="PL1:PN1"/>
+    <mergeCell ref="PL3:PN3"/>
+    <mergeCell ref="QD3:QF3"/>
+    <mergeCell ref="PO1:PQ1"/>
+    <mergeCell ref="PO3:PQ3"/>
+    <mergeCell ref="PR1:PT1"/>
+    <mergeCell ref="PR3:PT3"/>
+    <mergeCell ref="PU1:PW1"/>
+    <mergeCell ref="PU3:PW3"/>
     <mergeCell ref="QP1:QR1"/>
     <mergeCell ref="QP3:QR3"/>
     <mergeCell ref="QS1:QU1"/>
@@ -14455,79 +14530,6 @@
     <mergeCell ref="QA1:QC1"/>
     <mergeCell ref="QA3:QC3"/>
     <mergeCell ref="QD1:QF1"/>
-    <mergeCell ref="QD3:QF3"/>
-    <mergeCell ref="PO1:PQ1"/>
-    <mergeCell ref="PO3:PQ3"/>
-    <mergeCell ref="PR1:PT1"/>
-    <mergeCell ref="PR3:PT3"/>
-    <mergeCell ref="PU1:PW1"/>
-    <mergeCell ref="PU3:PW3"/>
-    <mergeCell ref="PF1:PH1"/>
-    <mergeCell ref="PF3:PH3"/>
-    <mergeCell ref="PI1:PK1"/>
-    <mergeCell ref="PI3:PK3"/>
-    <mergeCell ref="PL1:PN1"/>
-    <mergeCell ref="PL3:PN3"/>
-    <mergeCell ref="NG1:OY1"/>
-    <mergeCell ref="NG3:OY3"/>
-    <mergeCell ref="OZ1:PB1"/>
-    <mergeCell ref="OZ3:PB3"/>
-    <mergeCell ref="PC1:PE1"/>
-    <mergeCell ref="PC3:PE3"/>
-    <mergeCell ref="MC1:MN1"/>
-    <mergeCell ref="MC3:MN3"/>
-    <mergeCell ref="MO1:MT1"/>
-    <mergeCell ref="MO3:MT3"/>
-    <mergeCell ref="MU1:NF1"/>
-    <mergeCell ref="MU3:NF3"/>
-    <mergeCell ref="LE1:LJ1"/>
-    <mergeCell ref="LE3:LJ3"/>
-    <mergeCell ref="LK1:LV1"/>
-    <mergeCell ref="LK3:LV3"/>
-    <mergeCell ref="LW1:MB1"/>
-    <mergeCell ref="LW3:MB3"/>
-    <mergeCell ref="JU1:KF1"/>
-    <mergeCell ref="JU3:KF3"/>
-    <mergeCell ref="KG1:KR1"/>
-    <mergeCell ref="KG3:KR3"/>
-    <mergeCell ref="KS1:LD1"/>
-    <mergeCell ref="KS3:LD3"/>
-    <mergeCell ref="IK1:IV1"/>
-    <mergeCell ref="IK3:IV3"/>
-    <mergeCell ref="IW1:JH1"/>
-    <mergeCell ref="IW3:JH3"/>
-    <mergeCell ref="JI1:JT1"/>
-    <mergeCell ref="JI3:JT3"/>
-    <mergeCell ref="HA1:HL1"/>
-    <mergeCell ref="HA3:HL3"/>
-    <mergeCell ref="HM1:HX1"/>
-    <mergeCell ref="HM3:HX3"/>
-    <mergeCell ref="HY1:IJ1"/>
-    <mergeCell ref="HY3:IJ3"/>
-    <mergeCell ref="ES1:FP1"/>
-    <mergeCell ref="ES3:FP3"/>
-    <mergeCell ref="FQ1:GN1"/>
-    <mergeCell ref="FQ3:GN3"/>
-    <mergeCell ref="GO1:GZ1"/>
-    <mergeCell ref="GO3:GZ3"/>
-    <mergeCell ref="BY1:CV1"/>
-    <mergeCell ref="BY3:CV3"/>
-    <mergeCell ref="CW1:DT1"/>
-    <mergeCell ref="CW3:DT3"/>
-    <mergeCell ref="DU1:ER1"/>
-    <mergeCell ref="DU3:ER3"/>
-    <mergeCell ref="AF1:AT1"/>
-    <mergeCell ref="AF3:AT3"/>
-    <mergeCell ref="AU1:BI1"/>
-    <mergeCell ref="AU3:BI3"/>
-    <mergeCell ref="BJ1:BX1"/>
-    <mergeCell ref="BJ3:BX3"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="K1:S1"/>
-    <mergeCell ref="K3:S3"/>
-    <mergeCell ref="T1:AE1"/>
-    <mergeCell ref="T3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>